<commit_message>
clean up color scheme
</commit_message>
<xml_diff>
--- a/ANOSIM_sensitivity_FL.xlsx
+++ b/ANOSIM_sensitivity_FL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>manhattan</t>
   </si>
@@ -90,12 +90,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,9 +116,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -180,9 +189,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$J$2</c:f>
+              <c:f>Sheet1!$B$2:$L$2</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>manhattan</c:v>
                 </c:pt>
@@ -209,16 +218,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>kulczynski</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>raup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$J$3</c:f>
+              <c:f>Sheet1!$B$3:$L$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.1209353</c:v>
                 </c:pt>
@@ -245,6 +257,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.10038846999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.5291832222222216E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -284,9 +302,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$J$2</c:f>
+              <c:f>Sheet1!$B$2:$L$2</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>manhattan</c:v>
                 </c:pt>
@@ -313,16 +331,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>kulczynski</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>raup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$J$4</c:f>
+              <c:f>Sheet1!$B$4:$L$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.14942749999999999</c:v>
                 </c:pt>
@@ -349,6 +370,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.11463015</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.10886101777777779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -388,9 +415,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$J$2</c:f>
+              <c:f>Sheet1!$B$2:$L$2</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>manhattan</c:v>
                 </c:pt>
@@ -417,16 +444,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>kulczynski</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>raup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$J$5</c:f>
+              <c:f>Sheet1!$B$5:$L$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.31428850000000003</c:v>
                 </c:pt>
@@ -453,6 +483,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8.253779E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.2383511111111122E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,9 +528,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$J$2</c:f>
+              <c:f>Sheet1!$B$2:$L$2</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>manhattan</c:v>
                 </c:pt>
@@ -521,16 +557,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>kulczynski</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>raup</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$J$6</c:f>
+              <c:f>Sheet1!$B$6:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.203538</c:v>
                 </c:pt>
@@ -557,6 +596,12 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.13323436</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.11774665555555555</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -605,7 +650,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -764,7 +809,746 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>season</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$40:$L$40</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>manhattan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>canberra</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clark</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>bray</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>jaccard</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gower</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>horn</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>binomial</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>kulczynski</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>raup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$41:$L$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8.8381849999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5291050000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.2900980000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0684049999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0684049999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13006271999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7150530000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6495010000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.8316199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.5551826666666669E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-55E7-4451-B156-00C67B448201}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>marina</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$40:$L$40</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>manhattan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>canberra</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clark</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>bray</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>jaccard</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gower</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>horn</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>binomial</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>kulczynski</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>raup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$L$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4.8853599999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7248269999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3463329999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.9897260000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9897260000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8352530000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.145288E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.7013670000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.7910619999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.8232157777777755E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-55E7-4451-B156-00C67B448201}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>region</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$40:$L$40</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>manhattan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>canberra</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clark</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>bray</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>jaccard</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gower</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>horn</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>binomial</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>kulczynski</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>raup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$43:$L$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.10664009000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.858058E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.6499600000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1174649999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.1174649999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4212650000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8538349999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1624530000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.6887070000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.1703574444444441E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-55E7-4451-B156-00C67B448201}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>region2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$40:$L$40</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>manhattan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>canberra</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clark</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>bray</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>jaccard</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>gower</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>horn</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>binomial</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>kulczynski</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>raup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$44:$L$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.3971870000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.1187050000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10107292</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11503803</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11503803</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5607799999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10304153000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10748365999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11112171999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.3729178888888903E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-55E7-4451-B156-00C67B448201}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1721262735"/>
+        <c:axId val="1721269807"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1721262735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1721269807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1721269807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1721262735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1320,14 +2104,530 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>384810</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
@@ -1347,6 +2647,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1618,20 +2948,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1663,7 +2993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1697,8 +3027,12 @@
       <c r="K3">
         <v>0</v>
       </c>
+      <c r="L3">
+        <f>AVERAGE(B3:J3)</f>
+        <v>7.5291832222222216E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1732,8 +3066,12 @@
       <c r="K4">
         <v>0</v>
       </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L6" si="0">AVERAGE(B4:J4)</f>
+        <v>0.10886101777777779</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1767,8 +3105,12 @@
       <c r="K5">
         <v>0</v>
       </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>9.2383511111111122E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1802,8 +3144,12 @@
       <c r="K6">
         <v>0</v>
       </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.11774665555555555</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1E-3</v>
       </c>
@@ -1835,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1E-3</v>
       </c>
@@ -1867,7 +3213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>1E-3</v>
       </c>
@@ -1899,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>1E-3</v>
       </c>
@@ -1931,47 +3277,393 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>AVERAGE(B3:B6)</f>
         <v>0.197047325</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:K11" si="0">AVERAGE(C3:C6)</f>
+        <f t="shared" ref="C11:K11" si="1">AVERAGE(C3:C6)</f>
         <v>5.7152417499999997E-2</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.2660739999999998E-2</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14787207499999999</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14787207499999999</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1784412499999996E-2</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.5506267500000001E-2</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9543782499999994E-2</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1076976925</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>8.8381849999999998E-2</v>
+      </c>
+      <c r="C41">
+        <v>6.5291050000000003E-2</v>
+      </c>
+      <c r="D41">
+        <v>7.2900980000000004E-2</v>
+      </c>
+      <c r="E41">
+        <v>7.0684049999999998E-2</v>
+      </c>
+      <c r="F41">
+        <v>7.0684049999999998E-2</v>
+      </c>
+      <c r="G41">
+        <v>0.13006271999999999</v>
+      </c>
+      <c r="H41">
+        <v>4.7150530000000003E-2</v>
+      </c>
+      <c r="I41">
+        <v>7.6495010000000002E-2</v>
+      </c>
+      <c r="J41">
+        <v>5.8316199999999999E-2</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <f>AVERAGE(B41:J41)</f>
+        <v>7.5551826666666669E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42">
+        <v>4.8853599999999997E-2</v>
+      </c>
+      <c r="C42">
+        <v>6.7248269999999999E-2</v>
+      </c>
+      <c r="D42">
+        <v>7.3463329999999993E-2</v>
+      </c>
+      <c r="E42">
+        <v>8.9897260000000007E-2</v>
+      </c>
+      <c r="F42">
+        <v>8.9897260000000007E-2</v>
+      </c>
+      <c r="G42">
+        <v>7.8352530000000004E-2</v>
+      </c>
+      <c r="H42">
+        <v>9.145288E-2</v>
+      </c>
+      <c r="I42">
+        <v>7.7013670000000006E-2</v>
+      </c>
+      <c r="J42">
+        <v>8.7910619999999995E-2</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <f t="shared" ref="L42:L44" si="2">AVERAGE(B42:J42)</f>
+        <v>7.8232157777777755E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43">
+        <v>0.10664009000000001</v>
+      </c>
+      <c r="C43">
+        <v>5.858058E-2</v>
+      </c>
+      <c r="D43">
+        <v>6.6499600000000006E-2</v>
+      </c>
+      <c r="E43">
+        <v>9.1174649999999996E-2</v>
+      </c>
+      <c r="F43">
+        <v>9.1174649999999996E-2</v>
+      </c>
+      <c r="G43">
+        <v>7.4212650000000005E-2</v>
+      </c>
+      <c r="H43">
+        <v>9.8538349999999997E-2</v>
+      </c>
+      <c r="I43">
+        <v>7.1624530000000006E-2</v>
+      </c>
+      <c r="J43">
+        <v>7.6887070000000002E-2</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="2"/>
+        <v>8.1703574444444441E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>3.3971870000000001E-2</v>
+      </c>
+      <c r="C44">
+        <v>9.1187050000000006E-2</v>
+      </c>
+      <c r="D44">
+        <v>0.10107292</v>
+      </c>
+      <c r="E44">
+        <v>0.11503803</v>
+      </c>
+      <c r="F44">
+        <v>0.11503803</v>
+      </c>
+      <c r="G44">
+        <v>6.5607799999999994E-2</v>
+      </c>
+      <c r="H44">
+        <v>0.10304153000000001</v>
+      </c>
+      <c r="I44">
+        <v>0.10748365999999999</v>
+      </c>
+      <c r="J44">
+        <v>0.11112171999999999</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>9.3729178888888903E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>1E-3</v>
+      </c>
+      <c r="C45">
+        <v>1E-3</v>
+      </c>
+      <c r="D45">
+        <v>1E-3</v>
+      </c>
+      <c r="E45">
+        <v>1E-3</v>
+      </c>
+      <c r="F45">
+        <v>1E-3</v>
+      </c>
+      <c r="G45">
+        <v>1E-3</v>
+      </c>
+      <c r="H45">
+        <v>1E-3</v>
+      </c>
+      <c r="I45">
+        <v>1E-3</v>
+      </c>
+      <c r="J45">
+        <v>1E-3</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>1E-3</v>
+      </c>
+      <c r="C46">
+        <v>1E-3</v>
+      </c>
+      <c r="D46">
+        <v>1E-3</v>
+      </c>
+      <c r="E46">
+        <v>1E-3</v>
+      </c>
+      <c r="F46">
+        <v>1E-3</v>
+      </c>
+      <c r="G46">
+        <v>1E-3</v>
+      </c>
+      <c r="H46">
+        <v>1E-3</v>
+      </c>
+      <c r="I46">
+        <v>1E-3</v>
+      </c>
+      <c r="J46">
+        <v>1E-3</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>1E-3</v>
+      </c>
+      <c r="C47">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D47">
+        <v>2E-3</v>
+      </c>
+      <c r="E47">
+        <v>1E-3</v>
+      </c>
+      <c r="F47">
+        <v>1E-3</v>
+      </c>
+      <c r="G47">
+        <v>2E-3</v>
+      </c>
+      <c r="H47">
+        <v>1E-3</v>
+      </c>
+      <c r="I47">
+        <v>1E-3</v>
+      </c>
+      <c r="J47">
+        <v>1E-3</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>1E-3</v>
+      </c>
+      <c r="C48">
+        <v>1E-3</v>
+      </c>
+      <c r="D48">
+        <v>1E-3</v>
+      </c>
+      <c r="E48">
+        <v>1E-3</v>
+      </c>
+      <c r="F48">
+        <v>1E-3</v>
+      </c>
+      <c r="G48">
+        <v>1E-3</v>
+      </c>
+      <c r="H48">
+        <v>1E-3</v>
+      </c>
+      <c r="I48">
+        <v>1E-3</v>
+      </c>
+      <c r="J48">
+        <v>1E-3</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>